<commit_message>
Fixed data to match the data collected by Anderson and published by Fisher
</commit_message>
<xml_diff>
--- a/excel/iris.xlsx
+++ b/excel/iris.xlsx
@@ -58,6 +58,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -141,14 +142,14 @@
   </sheetPr>
   <dimension ref="A1:E151"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D39" activeCellId="0" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.03"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="9.35"/>
@@ -761,7 +762,7 @@
         <v>1.5</v>
       </c>
       <c r="D36" s="0" t="n">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="E36" s="0" t="s">
         <v>5</v>
@@ -806,13 +807,13 @@
         <v>4.9</v>
       </c>
       <c r="B39" s="0" t="n">
-        <v>3.1</v>
+        <v>3.6</v>
       </c>
       <c r="C39" s="0" t="n">
-        <v>1.5</v>
+        <v>1.4</v>
       </c>
       <c r="D39" s="0" t="n">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="E39" s="0" t="s">
         <v>5</v>

</xml_diff>